<commit_message>
sit lab 2 done
</commit_message>
<xml_diff>
--- a/sit/lab_2/Практика/zp1.xlsx
+++ b/sit/lab_2/Практика/zp1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F79E0768-50DF-4D18-ACEF-1F3381B840C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2446FDF6-BCA6-4460-940F-449B62E7CED1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{F79E0768-50DF-4D18-ACEF-1F3381B840C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4014CE5-74AB-40DA-9369-61E6124E0DB3}"/>
   <bookViews>
-    <workbookView xWindow="-10380" yWindow="3645" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3645" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
   <si>
     <t>Фамилия</t>
   </si>
@@ -132,15 +132,22 @@
   </si>
   <si>
     <t>Амосова</t>
+  </si>
+  <si>
+    <t>Количествое юбиляров</t>
+  </si>
+  <si>
+    <t>Количество человек моложе 30 лет</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot;р.&quot;"/>
     <numFmt numFmtId="165" formatCode="#,##0.00_р_."/>
+    <numFmt numFmtId="169" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -172,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -189,15 +196,25 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+        <strike val="0"/>
+        <color theme="3"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -882,10 +899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D12"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,17 +910,18 @@
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -932,12 +950,20 @@
       <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="8">
         <v>30317</v>
       </c>
       <c r="D3">
-        <f ca="1">INT((TODAY()-C3)/365)</f>
+        <f t="shared" ref="D3:D12" ca="1" si="0">INT((TODAY()-C3)/365)</f>
         <v>39</v>
+      </c>
+      <c r="E3" t="str">
+        <f ca="1">IF(MOD(D3,5)=0,"Юбилей","")</f>
+        <v/>
+      </c>
+      <c r="F3" s="10">
+        <f ca="1">IF(E3="Юбилей",50,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,12 +973,20 @@
       <c r="B4" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>28945</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D12" ca="1" si="0">INT((TODAY()-C4)/365)</f>
+        <f t="shared" ca="1" si="0"/>
         <v>43</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" ref="E4:E12" ca="1" si="1">IF(MOD(D4,5)=0,"Юбилей","")</f>
+        <v/>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" ref="F4:F14" ca="1" si="2">IF(E4="Юбилей",50,0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -962,13 +996,21 @@
       <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>29680</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
+      <c r="E5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -977,13 +1019,21 @@
       <c r="B6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>29585</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
+      <c r="E6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -992,13 +1042,21 @@
       <c r="B7" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>30139</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
+      <c r="E7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Юбилей</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1007,13 +1065,21 @@
       <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>29500</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
+      <c r="E8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1022,13 +1088,21 @@
       <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>29750</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
+      <c r="E9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F9" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1037,13 +1111,21 @@
       <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>29061</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
         <v>43</v>
       </c>
+      <c r="E10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F10" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1052,13 +1134,21 @@
       <c r="B11" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>29823</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
         <v>41</v>
       </c>
+      <c r="E11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F11" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1067,18 +1157,57 @@
       <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>29427</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
         <v>42</v>
       </c>
+      <c r="E12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="F12" s="10">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13">
+        <f ca="1">COUNTIF(E3:E12,"Юбилей")</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14">
+        <f ca="1">COUNTIF(D3:D12, "&lt; 30")</f>
+        <v>0</v>
+      </c>
+      <c r="F14" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
+  <conditionalFormatting sqref="E3:E14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Юбилей"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>

</xml_diff>